<commit_message>
addin remove project feature updated - should be functionality matched to addon from sheets
</commit_message>
<xml_diff>
--- a/sheets/Assets Repo.xlsx
+++ b/sheets/Assets Repo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\sb\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C92595-6448-4D6B-B0A2-797F684FAEE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CBC658-BF17-4820-A32B-433A1B63ABF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="3040" windowWidth="19200" windowHeight="10073" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6020" yWindow="3380" windowWidth="19200" windowHeight="10073" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
getting close on addin
</commit_message>
<xml_diff>
--- a/sheets/Assets Repo.xlsx
+++ b/sheets/Assets Repo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\sb\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E963A-6461-4B73-9168-6DBED70777D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE30496-5EE1-4E40-833C-B02CE9C0FCCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="3640" windowWidth="19200" windowHeight="10073" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4473" yWindow="1893" windowWidth="19200" windowHeight="10074" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>

</xml_diff>